<commit_message>
find half of tame pdfs
</commit_message>
<xml_diff>
--- a/tame/core_139/assessment_framework.xlsx
+++ b/tame/core_139/assessment_framework.xlsx
@@ -273,12 +273,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E19" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Book review</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E62" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Duplicate of 056</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="992" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="424">
   <si>
     <t>Substantive domain</t>
   </si>
@@ -1997,7 +2045,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5880,10 +5928,10 @@
   <dimension ref="A1:BB155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="AV6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="AE56" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="BA19" sqref="BA19"/>
+      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7114,8 +7162,8 @@
       <c r="D19" t="s">
         <v>224</v>
       </c>
-      <c r="E19" t="s">
-        <v>350</v>
+      <c r="E19">
+        <v>0</v>
       </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -7185,8 +7233,8 @@
       <c r="D20" t="s">
         <v>225</v>
       </c>
-      <c r="E20" t="s">
-        <v>350</v>
+      <c r="E20">
+        <v>1</v>
       </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -7256,8 +7304,8 @@
       <c r="D21" t="s">
         <v>226</v>
       </c>
-      <c r="E21" t="s">
-        <v>350</v>
+      <c r="E21">
+        <v>1</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -7327,8 +7375,8 @@
       <c r="D22" t="s">
         <v>227</v>
       </c>
-      <c r="E22" t="s">
-        <v>350</v>
+      <c r="E22">
+        <v>1</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -7398,8 +7446,8 @@
       <c r="D23" t="s">
         <v>228</v>
       </c>
-      <c r="E23" t="s">
-        <v>350</v>
+      <c r="E23">
+        <v>1</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -7469,8 +7517,8 @@
       <c r="D24" t="s">
         <v>229</v>
       </c>
-      <c r="E24" t="s">
-        <v>350</v>
+      <c r="E24">
+        <v>1</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -7540,8 +7588,8 @@
       <c r="D25" t="s">
         <v>230</v>
       </c>
-      <c r="E25" t="s">
-        <v>350</v>
+      <c r="E25">
+        <v>1</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -7611,8 +7659,8 @@
       <c r="D26" t="s">
         <v>231</v>
       </c>
-      <c r="E26" t="s">
-        <v>350</v>
+      <c r="E26">
+        <v>1</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -7682,8 +7730,8 @@
       <c r="D27" t="s">
         <v>232</v>
       </c>
-      <c r="E27" t="s">
-        <v>350</v>
+      <c r="E27">
+        <v>1</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -7753,8 +7801,8 @@
       <c r="D28" t="s">
         <v>233</v>
       </c>
-      <c r="E28" t="s">
-        <v>350</v>
+      <c r="E28">
+        <v>1</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -7824,8 +7872,8 @@
       <c r="D29" t="s">
         <v>234</v>
       </c>
-      <c r="E29" t="s">
-        <v>350</v>
+      <c r="E29">
+        <v>1</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -7895,8 +7943,8 @@
       <c r="D30" t="s">
         <v>235</v>
       </c>
-      <c r="E30" t="s">
-        <v>350</v>
+      <c r="E30">
+        <v>1</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -7966,8 +8014,8 @@
       <c r="D31" t="s">
         <v>236</v>
       </c>
-      <c r="E31" t="s">
-        <v>350</v>
+      <c r="E31">
+        <v>1</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -8037,8 +8085,8 @@
       <c r="D32" t="s">
         <v>228</v>
       </c>
-      <c r="E32" t="s">
-        <v>350</v>
+      <c r="E32">
+        <v>0</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
@@ -8108,8 +8156,8 @@
       <c r="D33" t="s">
         <v>237</v>
       </c>
-      <c r="E33" t="s">
-        <v>350</v>
+      <c r="E33">
+        <v>1</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
@@ -8179,8 +8227,8 @@
       <c r="D34" t="s">
         <v>238</v>
       </c>
-      <c r="E34" t="s">
-        <v>350</v>
+      <c r="E34">
+        <v>1</v>
       </c>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
@@ -8250,8 +8298,8 @@
       <c r="D35" t="s">
         <v>239</v>
       </c>
-      <c r="E35" t="s">
-        <v>350</v>
+      <c r="E35">
+        <v>1</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -8321,8 +8369,8 @@
       <c r="D36" t="s">
         <v>240</v>
       </c>
-      <c r="E36" t="s">
-        <v>350</v>
+      <c r="E36">
+        <v>0</v>
       </c>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
@@ -8392,8 +8440,8 @@
       <c r="D37" t="s">
         <v>227</v>
       </c>
-      <c r="E37" t="s">
-        <v>350</v>
+      <c r="E37">
+        <v>1</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
@@ -8463,8 +8511,8 @@
       <c r="D38" t="s">
         <v>241</v>
       </c>
-      <c r="E38" t="s">
-        <v>350</v>
+      <c r="E38">
+        <v>1</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
@@ -8534,8 +8582,8 @@
       <c r="D39" t="s">
         <v>242</v>
       </c>
-      <c r="E39" t="s">
-        <v>350</v>
+      <c r="E39">
+        <v>1</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
@@ -8605,8 +8653,8 @@
       <c r="D40" t="s">
         <v>243</v>
       </c>
-      <c r="E40" t="s">
-        <v>350</v>
+      <c r="E40">
+        <v>1</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
@@ -8676,8 +8724,8 @@
       <c r="D41" t="s">
         <v>227</v>
       </c>
-      <c r="E41" t="s">
-        <v>350</v>
+      <c r="E41">
+        <v>1</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -8747,8 +8795,8 @@
       <c r="D42" t="s">
         <v>244</v>
       </c>
-      <c r="E42" t="s">
-        <v>350</v>
+      <c r="E42">
+        <v>1</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -8818,8 +8866,8 @@
       <c r="D43" t="s">
         <v>245</v>
       </c>
-      <c r="E43" t="s">
-        <v>350</v>
+      <c r="E43">
+        <v>1</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -8889,8 +8937,8 @@
       <c r="D44" t="s">
         <v>246</v>
       </c>
-      <c r="E44" t="s">
-        <v>350</v>
+      <c r="E44">
+        <v>1</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
@@ -8960,8 +9008,8 @@
       <c r="D45" t="s">
         <v>244</v>
       </c>
-      <c r="E45" t="s">
-        <v>350</v>
+      <c r="E45">
+        <v>1</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
@@ -9031,8 +9079,8 @@
       <c r="D46" t="s">
         <v>247</v>
       </c>
-      <c r="E46" t="s">
-        <v>350</v>
+      <c r="E46">
+        <v>1</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
@@ -9102,8 +9150,8 @@
       <c r="D47" t="s">
         <v>248</v>
       </c>
-      <c r="E47" t="s">
-        <v>350</v>
+      <c r="E47">
+        <v>1</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
@@ -9173,8 +9221,8 @@
       <c r="D48" t="s">
         <v>249</v>
       </c>
-      <c r="E48" t="s">
-        <v>350</v>
+      <c r="E48">
+        <v>1</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2"/>
@@ -9244,8 +9292,8 @@
       <c r="D49" t="s">
         <v>250</v>
       </c>
-      <c r="E49" t="s">
-        <v>350</v>
+      <c r="E49">
+        <v>1</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -9315,8 +9363,8 @@
       <c r="D50" t="s">
         <v>251</v>
       </c>
-      <c r="E50" t="s">
-        <v>350</v>
+      <c r="E50">
+        <v>1</v>
       </c>
       <c r="F50" s="2"/>
       <c r="G50" s="2"/>
@@ -9386,8 +9434,8 @@
       <c r="D51" t="s">
         <v>252</v>
       </c>
-      <c r="E51" t="s">
-        <v>350</v>
+      <c r="E51">
+        <v>1</v>
       </c>
       <c r="F51" s="2"/>
       <c r="G51" s="2"/>
@@ -9457,8 +9505,8 @@
       <c r="D52" t="s">
         <v>253</v>
       </c>
-      <c r="E52" t="s">
-        <v>350</v>
+      <c r="E52">
+        <v>1</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -9528,8 +9576,8 @@
       <c r="D53" t="s">
         <v>254</v>
       </c>
-      <c r="E53" t="s">
-        <v>350</v>
+      <c r="E53">
+        <v>1</v>
       </c>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -9599,8 +9647,8 @@
       <c r="D54" t="s">
         <v>255</v>
       </c>
-      <c r="E54" t="s">
-        <v>350</v>
+      <c r="E54">
+        <v>1</v>
       </c>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -9670,8 +9718,8 @@
       <c r="D55" t="s">
         <v>244</v>
       </c>
-      <c r="E55" t="s">
-        <v>350</v>
+      <c r="E55">
+        <v>1</v>
       </c>
       <c r="F55" s="2"/>
       <c r="G55" s="2"/>
@@ -9741,8 +9789,8 @@
       <c r="D56" t="s">
         <v>256</v>
       </c>
-      <c r="E56" t="s">
-        <v>350</v>
+      <c r="E56">
+        <v>1</v>
       </c>
       <c r="F56" s="2"/>
       <c r="G56" s="2"/>
@@ -9812,8 +9860,8 @@
       <c r="D57" t="s">
         <v>257</v>
       </c>
-      <c r="E57" t="s">
-        <v>350</v>
+      <c r="E57">
+        <v>1</v>
       </c>
       <c r="F57" s="2"/>
       <c r="G57" s="2"/>
@@ -9883,8 +9931,8 @@
       <c r="D58" t="s">
         <v>258</v>
       </c>
-      <c r="E58" t="s">
-        <v>350</v>
+      <c r="E58">
+        <v>1</v>
       </c>
       <c r="F58" s="2"/>
       <c r="G58" s="2"/>
@@ -9954,8 +10002,8 @@
       <c r="D59" t="s">
         <v>244</v>
       </c>
-      <c r="E59" t="s">
-        <v>350</v>
+      <c r="E59">
+        <v>1</v>
       </c>
       <c r="F59" s="2"/>
       <c r="G59" s="2"/>
@@ -10025,8 +10073,8 @@
       <c r="D60" t="s">
         <v>259</v>
       </c>
-      <c r="E60" t="s">
-        <v>350</v>
+      <c r="E60">
+        <v>1</v>
       </c>
       <c r="F60" s="2"/>
       <c r="G60" s="2"/>
@@ -10096,8 +10144,8 @@
       <c r="D61" t="s">
         <v>260</v>
       </c>
-      <c r="E61" t="s">
-        <v>350</v>
+      <c r="E61">
+        <v>1</v>
       </c>
       <c r="F61" s="2"/>
       <c r="G61" s="2"/>
@@ -10167,8 +10215,8 @@
       <c r="D62" t="s">
         <v>260</v>
       </c>
-      <c r="E62" t="s">
-        <v>350</v>
+      <c r="E62">
+        <v>0</v>
       </c>
       <c r="F62" s="2"/>
       <c r="G62" s="2"/>
@@ -10238,8 +10286,8 @@
       <c r="D63" t="s">
         <v>261</v>
       </c>
-      <c r="E63" t="s">
-        <v>350</v>
+      <c r="E63">
+        <v>1</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2"/>
@@ -10309,8 +10357,8 @@
       <c r="D64" t="s">
         <v>262</v>
       </c>
-      <c r="E64" t="s">
-        <v>350</v>
+      <c r="E64">
+        <v>1</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -10380,8 +10428,8 @@
       <c r="D65" t="s">
         <v>244</v>
       </c>
-      <c r="E65" t="s">
-        <v>350</v>
+      <c r="E65">
+        <v>1</v>
       </c>
       <c r="F65" s="2"/>
       <c r="G65" s="2"/>
@@ -10451,8 +10499,8 @@
       <c r="D66" t="s">
         <v>263</v>
       </c>
-      <c r="E66" t="s">
-        <v>350</v>
+      <c r="E66">
+        <v>1</v>
       </c>
       <c r="F66" s="2"/>
       <c r="G66" s="2"/>
@@ -10522,8 +10570,8 @@
       <c r="D67" t="s">
         <v>264</v>
       </c>
-      <c r="E67" t="s">
-        <v>350</v>
+      <c r="E67">
+        <v>1</v>
       </c>
       <c r="F67" s="2"/>
       <c r="G67" s="2"/>
@@ -10593,8 +10641,8 @@
       <c r="D68" t="s">
         <v>265</v>
       </c>
-      <c r="E68" t="s">
-        <v>350</v>
+      <c r="E68">
+        <v>1</v>
       </c>
       <c r="F68" s="2"/>
       <c r="G68" s="2"/>
@@ -10664,8 +10712,8 @@
       <c r="D69" t="s">
         <v>266</v>
       </c>
-      <c r="E69" t="s">
-        <v>350</v>
+      <c r="E69">
+        <v>0</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2"/>
@@ -10735,8 +10783,8 @@
       <c r="D70" t="s">
         <v>267</v>
       </c>
-      <c r="E70" t="s">
-        <v>350</v>
+      <c r="E70">
+        <v>1</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2"/>
@@ -10806,8 +10854,8 @@
       <c r="D71" t="s">
         <v>268</v>
       </c>
-      <c r="E71" t="s">
-        <v>350</v>
+      <c r="E71">
+        <v>1</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2"/>
@@ -10877,8 +10925,8 @@
       <c r="D72" t="s">
         <v>269</v>
       </c>
-      <c r="E72" t="s">
-        <v>350</v>
+      <c r="E72">
+        <v>1</v>
       </c>
       <c r="F72" s="2"/>
       <c r="G72" s="2"/>
@@ -10948,8 +10996,8 @@
       <c r="D73" t="s">
         <v>270</v>
       </c>
-      <c r="E73" t="s">
-        <v>350</v>
+      <c r="E73">
+        <v>1</v>
       </c>
       <c r="F73" s="2"/>
       <c r="G73" s="2"/>
@@ -11019,8 +11067,8 @@
       <c r="D74" t="s">
         <v>262</v>
       </c>
-      <c r="E74" t="s">
-        <v>350</v>
+      <c r="E74">
+        <v>1</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2"/>
@@ -11090,8 +11138,8 @@
       <c r="D75" t="s">
         <v>271</v>
       </c>
-      <c r="E75" t="s">
-        <v>350</v>
+      <c r="E75">
+        <v>1</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2"/>

</xml_diff>

<commit_message>
find additional tame pdfs
</commit_message>
<xml_diff>
--- a/tame/core_139/assessment_framework.xlsx
+++ b/tame/core_139/assessment_framework.xlsx
@@ -321,12 +321,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="E90" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Book</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E103" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Book section</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="935" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="424">
   <si>
     <t>Substantive domain</t>
   </si>
@@ -2045,7 +2093,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5928,10 +5976,10 @@
   <dimension ref="A1:BB155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="AE56" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="AE95" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="E76" sqref="E76"/>
+      <selection pane="bottomRight" activeCell="AJ101" sqref="AJ101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11209,8 +11257,8 @@
       <c r="D76" t="s">
         <v>272</v>
       </c>
-      <c r="E76" t="s">
-        <v>350</v>
+      <c r="E76">
+        <v>1</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2"/>
@@ -11280,8 +11328,8 @@
       <c r="D77" t="s">
         <v>273</v>
       </c>
-      <c r="E77" t="s">
-        <v>350</v>
+      <c r="E77">
+        <v>1</v>
       </c>
       <c r="F77" s="2"/>
       <c r="G77" s="2"/>
@@ -11351,8 +11399,8 @@
       <c r="D78" t="s">
         <v>274</v>
       </c>
-      <c r="E78" t="s">
-        <v>350</v>
+      <c r="E78">
+        <v>1</v>
       </c>
       <c r="F78" s="2"/>
       <c r="G78" s="2"/>
@@ -11422,8 +11470,8 @@
       <c r="D79" t="s">
         <v>224</v>
       </c>
-      <c r="E79" t="s">
-        <v>350</v>
+      <c r="E79">
+        <v>1</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
@@ -11493,8 +11541,8 @@
       <c r="D80" t="s">
         <v>275</v>
       </c>
-      <c r="E80" t="s">
-        <v>350</v>
+      <c r="E80">
+        <v>1</v>
       </c>
       <c r="F80" s="2"/>
       <c r="G80" s="2"/>
@@ -11564,8 +11612,8 @@
       <c r="D81" t="s">
         <v>276</v>
       </c>
-      <c r="E81" t="s">
-        <v>350</v>
+      <c r="E81">
+        <v>0</v>
       </c>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
@@ -11635,8 +11683,8 @@
       <c r="D82" t="s">
         <v>277</v>
       </c>
-      <c r="E82" t="s">
-        <v>350</v>
+      <c r="E82">
+        <v>1</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
@@ -11706,8 +11754,8 @@
       <c r="D83" t="s">
         <v>278</v>
       </c>
-      <c r="E83" t="s">
-        <v>350</v>
+      <c r="E83">
+        <v>1</v>
       </c>
       <c r="F83" s="2"/>
       <c r="G83" s="2"/>
@@ -11777,8 +11825,8 @@
       <c r="D84" t="s">
         <v>279</v>
       </c>
-      <c r="E84" t="s">
-        <v>350</v>
+      <c r="E84">
+        <v>1</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2"/>
@@ -11848,8 +11896,8 @@
       <c r="D85" t="s">
         <v>280</v>
       </c>
-      <c r="E85" t="s">
-        <v>350</v>
+      <c r="E85">
+        <v>1</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2"/>
@@ -11919,8 +11967,8 @@
       <c r="D86" t="s">
         <v>259</v>
       </c>
-      <c r="E86" t="s">
-        <v>350</v>
+      <c r="E86">
+        <v>1</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2"/>
@@ -11990,8 +12038,8 @@
       <c r="D87" t="s">
         <v>281</v>
       </c>
-      <c r="E87" t="s">
-        <v>350</v>
+      <c r="E87">
+        <v>1</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
@@ -12061,8 +12109,8 @@
       <c r="D88" t="s">
         <v>269</v>
       </c>
-      <c r="E88" t="s">
-        <v>350</v>
+      <c r="E88">
+        <v>1</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2"/>
@@ -12132,8 +12180,8 @@
       <c r="D89" t="s">
         <v>282</v>
       </c>
-      <c r="E89" t="s">
-        <v>350</v>
+      <c r="E89">
+        <v>1</v>
       </c>
       <c r="F89" s="2"/>
       <c r="G89" s="2"/>
@@ -12203,8 +12251,8 @@
       <c r="D90" t="s">
         <v>283</v>
       </c>
-      <c r="E90" t="s">
-        <v>350</v>
+      <c r="E90">
+        <v>0</v>
       </c>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
@@ -12274,8 +12322,8 @@
       <c r="D91" t="s">
         <v>284</v>
       </c>
-      <c r="E91" t="s">
-        <v>350</v>
+      <c r="E91">
+        <v>1</v>
       </c>
       <c r="F91" s="2"/>
       <c r="G91" s="2"/>
@@ -12345,8 +12393,8 @@
       <c r="D92" t="s">
         <v>285</v>
       </c>
-      <c r="E92" t="s">
-        <v>350</v>
+      <c r="E92">
+        <v>1</v>
       </c>
       <c r="F92" s="2"/>
       <c r="G92" s="2"/>
@@ -12416,8 +12464,8 @@
       <c r="D93" t="s">
         <v>286</v>
       </c>
-      <c r="E93" t="s">
-        <v>350</v>
+      <c r="E93">
+        <v>1</v>
       </c>
       <c r="F93" s="2"/>
       <c r="G93" s="2"/>
@@ -12487,8 +12535,8 @@
       <c r="D94" t="s">
         <v>287</v>
       </c>
-      <c r="E94" t="s">
-        <v>350</v>
+      <c r="E94">
+        <v>1</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2"/>
@@ -12558,8 +12606,8 @@
       <c r="D95" t="s">
         <v>288</v>
       </c>
-      <c r="E95" t="s">
-        <v>350</v>
+      <c r="E95">
+        <v>1</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2"/>
@@ -12629,8 +12677,8 @@
       <c r="D96" t="s">
         <v>289</v>
       </c>
-      <c r="E96" t="s">
-        <v>350</v>
+      <c r="E96">
+        <v>1</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2"/>
@@ -12700,8 +12748,8 @@
       <c r="D97" t="s">
         <v>290</v>
       </c>
-      <c r="E97" t="s">
-        <v>350</v>
+      <c r="E97">
+        <v>1</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2"/>
@@ -12771,8 +12819,8 @@
       <c r="D98" t="s">
         <v>291</v>
       </c>
-      <c r="E98" t="s">
-        <v>350</v>
+      <c r="E98">
+        <v>1</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
@@ -12842,8 +12890,8 @@
       <c r="D99" t="s">
         <v>292</v>
       </c>
-      <c r="E99" t="s">
-        <v>350</v>
+      <c r="E99">
+        <v>1</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
@@ -12913,8 +12961,8 @@
       <c r="D100" t="s">
         <v>293</v>
       </c>
-      <c r="E100" t="s">
-        <v>350</v>
+      <c r="E100">
+        <v>1</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2"/>
@@ -12984,8 +13032,8 @@
       <c r="D101" t="s">
         <v>294</v>
       </c>
-      <c r="E101" t="s">
-        <v>350</v>
+      <c r="E101">
+        <v>1</v>
       </c>
       <c r="F101" s="2"/>
       <c r="G101" s="2"/>
@@ -13055,8 +13103,8 @@
       <c r="D102" t="s">
         <v>269</v>
       </c>
-      <c r="E102" t="s">
-        <v>350</v>
+      <c r="E102">
+        <v>1</v>
       </c>
       <c r="F102" s="2"/>
       <c r="G102" s="2"/>
@@ -13126,8 +13174,8 @@
       <c r="D103" t="s">
         <v>295</v>
       </c>
-      <c r="E103" t="s">
-        <v>350</v>
+      <c r="E103">
+        <v>0</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2"/>
@@ -13197,8 +13245,8 @@
       <c r="D104" t="s">
         <v>296</v>
       </c>
-      <c r="E104" t="s">
-        <v>350</v>
+      <c r="E104">
+        <v>0</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2"/>
@@ -13268,8 +13316,8 @@
       <c r="D105" t="s">
         <v>297</v>
       </c>
-      <c r="E105" t="s">
-        <v>350</v>
+      <c r="E105">
+        <v>1</v>
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2"/>

</xml_diff>

<commit_message>
find last tame pdfs
</commit_message>
<xml_diff>
--- a/tame/core_139/assessment_framework.xlsx
+++ b/tame/core_139/assessment_framework.xlsx
@@ -369,12 +369,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="E112" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Book section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E126" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+html page</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E144" authorId="2">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>jm383x:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+html download</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="866" uniqueCount="423">
   <si>
     <t>Substantive domain</t>
   </si>
@@ -1424,9 +1496,6 @@
   </si>
   <si>
     <t>[full reference at end]</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>score each reference and note all measures clearly defined</t>
@@ -2093,7 +2162,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2155,23 +2224,23 @@
         <v>344</v>
       </c>
       <c r="B11" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B13" t="s">
         <v>352</v>
-      </c>
-      <c r="B13" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
+        <v>381</v>
+      </c>
+      <c r="B15" t="s">
         <v>382</v>
-      </c>
-      <c r="B15" t="s">
-        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -5976,10 +6045,10 @@
   <dimension ref="A1:BB155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="5" ySplit="5" topLeftCell="AE95" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="5" topLeftCell="F6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="AJ101" sqref="AJ101"/>
+      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6012,7 +6081,7 @@
   <sheetData>
     <row r="1" spans="1:54">
       <c r="B1" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C1" s="1"/>
     </row>
@@ -6111,13 +6180,13 @@
     </row>
     <row r="5" spans="1:54" s="5" customFormat="1" ht="51">
       <c r="A5" s="5" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>349</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="F5" s="5" t="s">
         <v>345</v>
@@ -6159,7 +6228,7 @@
       </c>
       <c r="U5" s="8"/>
       <c r="V5" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="W5" s="5" t="s">
         <v>30</v>
@@ -6198,16 +6267,16 @@
         <v>16</v>
       </c>
       <c r="AK5" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="AL5" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="AM5" s="5" t="s">
         <v>360</v>
       </c>
-      <c r="AM5" s="5" t="s">
-        <v>361</v>
-      </c>
       <c r="AN5" s="5" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="AO5" s="5" t="s">
         <v>17</v>
@@ -6341,7 +6410,7 @@
         <v>127</v>
       </c>
       <c r="BB6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="7" spans="1:54">
@@ -13387,8 +13456,8 @@
       <c r="D106" t="s">
         <v>298</v>
       </c>
-      <c r="E106" t="s">
-        <v>350</v>
+      <c r="E106">
+        <v>1</v>
       </c>
       <c r="F106" s="2"/>
       <c r="G106" s="2"/>
@@ -13458,8 +13527,8 @@
       <c r="D107" t="s">
         <v>299</v>
       </c>
-      <c r="E107" t="s">
-        <v>350</v>
+      <c r="E107">
+        <v>1</v>
       </c>
       <c r="F107" s="2"/>
       <c r="G107" s="2"/>
@@ -13529,8 +13598,8 @@
       <c r="D108" t="s">
         <v>300</v>
       </c>
-      <c r="E108" t="s">
-        <v>350</v>
+      <c r="E108">
+        <v>1</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2"/>
@@ -13600,8 +13669,8 @@
       <c r="D109" t="s">
         <v>301</v>
       </c>
-      <c r="E109" t="s">
-        <v>350</v>
+      <c r="E109">
+        <v>1</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2"/>
@@ -13671,8 +13740,8 @@
       <c r="D110" t="s">
         <v>269</v>
       </c>
-      <c r="E110" t="s">
-        <v>350</v>
+      <c r="E110">
+        <v>1</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2"/>
@@ -13742,8 +13811,8 @@
       <c r="D111" t="s">
         <v>302</v>
       </c>
-      <c r="E111" t="s">
-        <v>350</v>
+      <c r="E111">
+        <v>1</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2"/>
@@ -13813,8 +13882,8 @@
       <c r="D112" t="s">
         <v>303</v>
       </c>
-      <c r="E112" t="s">
-        <v>350</v>
+      <c r="E112">
+        <v>0</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2"/>
@@ -13884,8 +13953,8 @@
       <c r="D113" t="s">
         <v>304</v>
       </c>
-      <c r="E113" t="s">
-        <v>350</v>
+      <c r="E113">
+        <v>1</v>
       </c>
       <c r="F113" s="2"/>
       <c r="G113" s="2"/>
@@ -13955,8 +14024,8 @@
       <c r="D114" t="s">
         <v>305</v>
       </c>
-      <c r="E114" t="s">
-        <v>350</v>
+      <c r="E114">
+        <v>1</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2"/>
@@ -14026,8 +14095,8 @@
       <c r="D115" t="s">
         <v>306</v>
       </c>
-      <c r="E115" t="s">
-        <v>350</v>
+      <c r="E115">
+        <v>1</v>
       </c>
       <c r="F115" s="2"/>
       <c r="G115" s="2"/>
@@ -14097,8 +14166,8 @@
       <c r="D116" t="s">
         <v>307</v>
       </c>
-      <c r="E116" t="s">
-        <v>350</v>
+      <c r="E116">
+        <v>1</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2"/>
@@ -14168,8 +14237,8 @@
       <c r="D117" t="s">
         <v>308</v>
       </c>
-      <c r="E117" t="s">
-        <v>350</v>
+      <c r="E117">
+        <v>1</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2"/>
@@ -14239,8 +14308,8 @@
       <c r="D118" t="s">
         <v>309</v>
       </c>
-      <c r="E118" t="s">
-        <v>350</v>
+      <c r="E118">
+        <v>1</v>
       </c>
       <c r="F118" s="2"/>
       <c r="G118" s="2"/>
@@ -14310,8 +14379,8 @@
       <c r="D119" t="s">
         <v>310</v>
       </c>
-      <c r="E119" t="s">
-        <v>350</v>
+      <c r="E119">
+        <v>1</v>
       </c>
       <c r="F119" s="2"/>
       <c r="G119" s="2"/>
@@ -14381,8 +14450,8 @@
       <c r="D120" t="s">
         <v>311</v>
       </c>
-      <c r="E120" t="s">
-        <v>350</v>
+      <c r="E120">
+        <v>1</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -14452,8 +14521,8 @@
       <c r="D121" t="s">
         <v>264</v>
       </c>
-      <c r="E121" t="s">
-        <v>350</v>
+      <c r="E121">
+        <v>1</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" s="2"/>
@@ -14523,8 +14592,8 @@
       <c r="D122" t="s">
         <v>312</v>
       </c>
-      <c r="E122" t="s">
-        <v>350</v>
+      <c r="E122">
+        <v>1</v>
       </c>
       <c r="F122" s="2"/>
       <c r="G122" s="2"/>
@@ -14594,8 +14663,8 @@
       <c r="D123" t="s">
         <v>313</v>
       </c>
-      <c r="E123" t="s">
-        <v>350</v>
+      <c r="E123">
+        <v>0</v>
       </c>
       <c r="F123" s="2"/>
       <c r="G123" s="2"/>
@@ -14665,8 +14734,8 @@
       <c r="D124" t="s">
         <v>314</v>
       </c>
-      <c r="E124" t="s">
-        <v>350</v>
+      <c r="E124">
+        <v>1</v>
       </c>
       <c r="F124" s="2"/>
       <c r="G124" s="2"/>
@@ -14736,8 +14805,8 @@
       <c r="D125" t="s">
         <v>315</v>
       </c>
-      <c r="E125" t="s">
-        <v>350</v>
+      <c r="E125">
+        <v>1</v>
       </c>
       <c r="F125" s="2"/>
       <c r="G125" s="2"/>
@@ -14807,8 +14876,8 @@
       <c r="D126" t="s">
         <v>316</v>
       </c>
-      <c r="E126" t="s">
-        <v>350</v>
+      <c r="E126">
+        <v>1</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="2"/>
@@ -14878,8 +14947,8 @@
       <c r="D127" t="s">
         <v>317</v>
       </c>
-      <c r="E127" t="s">
-        <v>350</v>
+      <c r="E127">
+        <v>1</v>
       </c>
       <c r="F127" s="2"/>
       <c r="G127" s="2"/>
@@ -14949,8 +15018,8 @@
       <c r="D128" t="s">
         <v>318</v>
       </c>
-      <c r="E128" t="s">
-        <v>350</v>
+      <c r="E128">
+        <v>1</v>
       </c>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
@@ -15020,8 +15089,8 @@
       <c r="D129" t="s">
         <v>319</v>
       </c>
-      <c r="E129" t="s">
-        <v>350</v>
+      <c r="E129">
+        <v>0</v>
       </c>
       <c r="F129" s="2"/>
       <c r="G129" s="2"/>
@@ -15091,8 +15160,8 @@
       <c r="D130" t="s">
         <v>320</v>
       </c>
-      <c r="E130" t="s">
-        <v>350</v>
+      <c r="E130">
+        <v>1</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -15162,8 +15231,8 @@
       <c r="D131" t="s">
         <v>321</v>
       </c>
-      <c r="E131" t="s">
-        <v>350</v>
+      <c r="E131">
+        <v>1</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2"/>
@@ -15233,8 +15302,8 @@
       <c r="D132" t="s">
         <v>322</v>
       </c>
-      <c r="E132" t="s">
-        <v>350</v>
+      <c r="E132">
+        <v>0</v>
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2"/>
@@ -15304,8 +15373,8 @@
       <c r="D133" t="s">
         <v>323</v>
       </c>
-      <c r="E133" t="s">
-        <v>350</v>
+      <c r="E133">
+        <v>1</v>
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2"/>
@@ -15375,8 +15444,8 @@
       <c r="D134" t="s">
         <v>324</v>
       </c>
-      <c r="E134" t="s">
-        <v>350</v>
+      <c r="E134">
+        <v>1</v>
       </c>
       <c r="F134" s="2"/>
       <c r="G134" s="2"/>
@@ -15446,8 +15515,8 @@
       <c r="D135" t="s">
         <v>325</v>
       </c>
-      <c r="E135" t="s">
-        <v>350</v>
+      <c r="E135">
+        <v>1</v>
       </c>
       <c r="F135" s="2"/>
       <c r="G135" s="2"/>
@@ -15517,8 +15586,8 @@
       <c r="D136" t="s">
         <v>326</v>
       </c>
-      <c r="E136" t="s">
-        <v>350</v>
+      <c r="E136">
+        <v>1</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2"/>
@@ -15588,8 +15657,8 @@
       <c r="D137" t="s">
         <v>327</v>
       </c>
-      <c r="E137" t="s">
-        <v>350</v>
+      <c r="E137">
+        <v>0</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -15659,8 +15728,8 @@
       <c r="D138" t="s">
         <v>328</v>
       </c>
-      <c r="E138" t="s">
-        <v>350</v>
+      <c r="E138">
+        <v>1</v>
       </c>
       <c r="F138" s="2"/>
       <c r="G138" s="2"/>
@@ -15730,8 +15799,8 @@
       <c r="D139" t="s">
         <v>227</v>
       </c>
-      <c r="E139" t="s">
-        <v>350</v>
+      <c r="E139">
+        <v>1</v>
       </c>
       <c r="F139" s="2"/>
       <c r="G139" s="2"/>
@@ -15801,8 +15870,8 @@
       <c r="D140" t="s">
         <v>329</v>
       </c>
-      <c r="E140" t="s">
-        <v>350</v>
+      <c r="E140">
+        <v>1</v>
       </c>
       <c r="F140" s="2"/>
       <c r="G140" s="2"/>
@@ -15872,8 +15941,8 @@
       <c r="D141" t="s">
         <v>330</v>
       </c>
-      <c r="E141" t="s">
-        <v>350</v>
+      <c r="E141">
+        <v>1</v>
       </c>
       <c r="F141" s="2"/>
       <c r="G141" s="2"/>
@@ -15943,8 +16012,8 @@
       <c r="D142" t="s">
         <v>331</v>
       </c>
-      <c r="E142" t="s">
-        <v>350</v>
+      <c r="E142">
+        <v>0</v>
       </c>
       <c r="F142" s="2"/>
       <c r="G142" s="2"/>
@@ -16014,8 +16083,8 @@
       <c r="D143" t="s">
         <v>332</v>
       </c>
-      <c r="E143" t="s">
-        <v>350</v>
+      <c r="E143">
+        <v>1</v>
       </c>
       <c r="F143" s="2"/>
       <c r="G143" s="2"/>
@@ -16085,8 +16154,8 @@
       <c r="D144" t="s">
         <v>333</v>
       </c>
-      <c r="E144" t="s">
-        <v>350</v>
+      <c r="E144">
+        <v>1</v>
       </c>
       <c r="F144" s="2"/>
       <c r="G144" s="2"/>
@@ -16750,19 +16819,19 @@
         <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16.5" customHeight="1">
@@ -16782,18 +16851,18 @@
         <v>284</v>
       </c>
       <c r="G4" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H4" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="5" spans="1:8">
       <c r="B5" t="s">
+        <v>363</v>
+      </c>
+      <c r="D5" t="s">
         <v>364</v>
-      </c>
-      <c r="D5" t="s">
-        <v>365</v>
       </c>
       <c r="E5" t="s">
         <v>40</v>
@@ -16802,21 +16871,21 @@
         <v>285</v>
       </c>
       <c r="G5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="6" spans="1:8">
       <c r="B6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C6" t="s">
+        <v>368</v>
+      </c>
+      <c r="D6" t="s">
         <v>369</v>
-      </c>
-      <c r="D6" t="s">
-        <v>370</v>
       </c>
       <c r="E6" t="s">
         <v>40</v>
@@ -16825,15 +16894,15 @@
         <v>285</v>
       </c>
       <c r="G6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="B7" t="s">
+        <v>371</v>
+      </c>
+      <c r="D7" t="s">
         <v>372</v>
-      </c>
-      <c r="D7" t="s">
-        <v>373</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -16842,21 +16911,21 @@
         <v>286</v>
       </c>
       <c r="G7" t="s">
+        <v>373</v>
+      </c>
+      <c r="H7" t="s">
         <v>374</v>
-      </c>
-      <c r="H7" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B11" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D11" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E11" t="s">
         <v>40</v>
@@ -16865,15 +16934,15 @@
         <v>288</v>
       </c>
       <c r="G11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="B12" t="s">
+        <v>386</v>
+      </c>
+      <c r="D12" t="s">
         <v>387</v>
-      </c>
-      <c r="D12" t="s">
-        <v>388</v>
       </c>
       <c r="E12" t="s">
         <v>40</v>
@@ -16882,15 +16951,15 @@
         <v>288</v>
       </c>
       <c r="G12" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="B13" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D13" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -16899,21 +16968,21 @@
         <v>289</v>
       </c>
       <c r="G13" t="s">
+        <v>390</v>
+      </c>
+      <c r="H13" t="s">
         <v>391</v>
-      </c>
-      <c r="H13" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B17" t="s">
+        <v>392</v>
+      </c>
+      <c r="D17" t="s">
         <v>393</v>
-      </c>
-      <c r="D17" t="s">
-        <v>394</v>
       </c>
       <c r="E17" t="s">
         <v>40</v>
@@ -16922,15 +16991,15 @@
         <v>289</v>
       </c>
       <c r="G17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="B18" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E18" t="s">
         <v>40</v>
@@ -16939,15 +17008,15 @@
         <v>290</v>
       </c>
       <c r="G18" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="B19" t="s">
+        <v>396</v>
+      </c>
+      <c r="D19" t="s">
         <v>397</v>
-      </c>
-      <c r="D19" t="s">
-        <v>398</v>
       </c>
       <c r="E19" t="s">
         <v>40</v>
@@ -16956,18 +17025,18 @@
         <v>291</v>
       </c>
       <c r="G19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
+        <v>399</v>
+      </c>
+      <c r="B23" t="s">
+        <v>399</v>
+      </c>
+      <c r="D23" t="s">
         <v>400</v>
-      </c>
-      <c r="B23" t="s">
-        <v>400</v>
-      </c>
-      <c r="D23" t="s">
-        <v>401</v>
       </c>
       <c r="E23" t="s">
         <v>40</v>
@@ -16976,15 +17045,15 @@
         <v>292</v>
       </c>
       <c r="G23" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="B24" t="s">
+        <v>402</v>
+      </c>
+      <c r="D24" t="s">
         <v>403</v>
-      </c>
-      <c r="D24" t="s">
-        <v>404</v>
       </c>
       <c r="E24" t="s">
         <v>40</v>
@@ -16993,15 +17062,15 @@
         <v>292</v>
       </c>
       <c r="G24" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="B25" t="s">
+        <v>404</v>
+      </c>
+      <c r="D25" t="s">
         <v>405</v>
-      </c>
-      <c r="D25" t="s">
-        <v>406</v>
       </c>
       <c r="E25" t="s">
         <v>40</v>
@@ -17010,18 +17079,18 @@
         <v>293</v>
       </c>
       <c r="G25" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B29" t="s">
+        <v>408</v>
+      </c>
+      <c r="D29" t="s">
         <v>409</v>
-      </c>
-      <c r="D29" t="s">
-        <v>410</v>
       </c>
       <c r="E29" t="s">
         <v>40</v>
@@ -17030,15 +17099,15 @@
         <v>294</v>
       </c>
       <c r="G29" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="B30" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D30" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E30" t="s">
         <v>40</v>
@@ -17047,15 +17116,15 @@
         <v>295</v>
       </c>
       <c r="G30" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="B31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D31" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E31" t="s">
         <v>40</v>
@@ -17064,15 +17133,15 @@
         <v>295</v>
       </c>
       <c r="G31" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="B32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D32" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E32" t="s">
         <v>40</v>
@@ -17081,15 +17150,15 @@
         <v>296</v>
       </c>
       <c r="G32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="2:7" s="20" customFormat="1">
       <c r="B33" s="20" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E33" s="20" t="s">
         <v>40</v>
@@ -17098,7 +17167,7 @@
         <v>297</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
   </sheetData>
@@ -17121,30 +17190,30 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="B4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="B5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="B6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
   </sheetData>

</xml_diff>